<commit_message>
add requirement.txt file, add convertion from lower case to upper case, add volume warning, add GROOT file
</commit_message>
<xml_diff>
--- a/work_load.xlsx
+++ b/work_load.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tomato Project\TomatoProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C2D19E-3B4A-43A0-8160-C0D8C51933F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED60066-F348-443C-9529-21F3E6A64A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="43200" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,26 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Two SQL Query</t>
-  </si>
-  <si>
-    <t>ER Diagram</t>
-  </si>
-  <si>
-    <t>Logic Diagram</t>
-  </si>
-  <si>
-    <t>Datalog</t>
-  </si>
-  <si>
-    <t>Theory</t>
-  </si>
-  <si>
-    <t>One SQL Query</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,10 +341,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C5" sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,32 +353,7 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix double message, add ending message
</commit_message>
<xml_diff>
--- a/work_load.xlsx
+++ b/work_load.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tomato Project\TomatoProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED60066-F348-443C-9529-21F3E6A64A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC07710-318C-4752-A11B-C77C01605D07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="43200" windowHeight="23445" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>2 Query SQL</t>
+  </si>
+  <si>
+    <t>Diagramma ER</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -341,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="A1:C5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -353,7 +360,16 @@
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>